<commit_message>
added two test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Freemium_Workspace\freemium\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soujanya\git\TechnavioLive\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCCC3DA-4522-472E-A4A6-6A8CAFB7D6E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC3B91-7BC9-48E5-B863-54E5BC681522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Offline</t>
-  </si>
-  <si>
     <t>TC001_POST_Request</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Infi123</t>
+  </si>
+  <si>
+    <t>Online</t>
   </si>
 </sst>
 </file>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE44068-76DD-46D6-BA08-F84E1EA9C793}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +777,7 @@
         <v>35</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C43D8AC-31DA-4A63-A5A1-CD94CEB8B5A1}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,42 +812,42 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>